<commit_message>
todo update and progress
</commit_message>
<xml_diff>
--- a/doc/doc_todo.xlsx
+++ b/doc/doc_todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="7215" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="asis" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="132">
   <si>
     <t>file</t>
   </si>
@@ -388,6 +389,30 @@
   </si>
   <si>
     <t>plot_fit(model, [type(s)], emp_priors, with_data, with_ui, axes, fig_size)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>graphics.plot_data_bars(df, style, color)</t>
+  </si>
+  <si>
+    <t>graphics.plot_data_bars(df, style, color, label)</t>
+  </si>
+  <si>
+    <t>delete data.plot_effects</t>
+  </si>
+  <si>
+    <t>delete plotting in other functions</t>
+  </si>
+  <si>
+    <t>delete data.vars.plot_trace</t>
+  </si>
+  <si>
+    <t>delete data.vars.plot_acorr</t>
+  </si>
+  <si>
+    <t>graphics.plot_convergence_diag(vars) -&gt; graphics.plot_acorr(vars)</t>
   </si>
 </sst>
 </file>
@@ -763,8 +788,8 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,72 +1503,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B15"/>
+  <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of todo list
</commit_message>
<xml_diff>
--- a/doc/doc_todo.xlsx
+++ b/doc/doc_todo.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="7215" windowHeight="8190"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="7215" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="asis" sheetId="1" r:id="rId1"/>
     <sheet name="todo" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="concerns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
   <si>
     <t>file</t>
   </si>
@@ -214,18 +214,12 @@
     <t>rename (plot_acorr)</t>
   </si>
   <si>
-    <t>viz_func options</t>
-  </si>
-  <si>
     <t>labels, options</t>
   </si>
   <si>
     <t>refactor into plot_fit</t>
   </si>
   <si>
-    <t>crashes frequently, one param at time?</t>
-  </si>
-  <si>
     <t>very similar to summarize_fit, refactor?</t>
   </si>
   <si>
@@ -413,6 +407,42 @@
   </si>
   <si>
     <t>new plot_fit makes this redundant; (vars[t],t) redundant, needs more options</t>
+  </si>
+  <si>
+    <t>viz_func options docs</t>
+  </si>
+  <si>
+    <t>crashes frequently, one param at time is redundant with all_plots_for</t>
+  </si>
+  <si>
+    <t>tests/test_data.py passes</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>concern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit.fit_consistent &lt;- fit_model.fit_consistent_model </t>
+  </si>
+  <si>
+    <t>fit.fit_asr &lt;-fit_module.fit_asr</t>
+  </si>
+  <si>
+    <t>ism.age_specific_rate &lt;- data_model.data_model</t>
+  </si>
+  <si>
+    <t>record reference values in model</t>
+  </si>
+  <si>
+    <t>expose interface for alternate rate_types as well as other outputs</t>
+  </si>
+  <si>
+    <t>docstring</t>
+  </si>
+  <si>
+    <t>delete data_model.py</t>
   </si>
 </sst>
 </file>
@@ -436,7 +466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -492,6 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,9 +832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1034,7 @@
       <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G21" t="s">
@@ -1008,7 +1045,7 @@
       <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G22" t="s">
@@ -1071,7 +1108,7 @@
       <c r="B30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G30" t="s">
@@ -1082,7 +1119,7 @@
       <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G31" t="s">
@@ -1091,62 +1128,62 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
         <v>92</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
         <v>93</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
@@ -1154,18 +1191,18 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E43" t="s">
         <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1175,7 +1212,7 @@
       <c r="B49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G49" t="s">
@@ -1186,22 +1223,22 @@
       <c r="B50" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="F51" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,7 +1257,7 @@
         <v>14</v>
       </c>
       <c r="G53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="G54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1253,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,7 +1308,7 @@
       <c r="B58" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G58" t="s">
@@ -1286,14 +1323,14 @@
         <v>14</v>
       </c>
       <c r="G59" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G60" t="s">
@@ -1323,30 +1360,30 @@
       <c r="B63" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
@@ -1354,7 +1391,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
         <v>14</v>
@@ -1362,7 +1399,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C68" t="s">
         <v>14</v>
@@ -1370,7 +1407,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C69" t="s">
         <v>14</v>
@@ -1378,40 +1415,40 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G72" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C73" t="s">
         <v>14</v>
@@ -1419,10 +1456,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C75" t="s">
         <v>14</v>
@@ -1430,24 +1467,24 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" t="s">
         <v>83</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>14</v>
@@ -1458,12 +1495,12 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -1474,33 +1511,33 @@
         <v>14</v>
       </c>
       <c r="G82" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -1514,20 +1551,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1535,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,7 +1580,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,15 +1588,15 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1567,7 +1604,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,15 +1612,15 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1599,7 +1636,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,15 +1644,15 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1623,23 +1660,23 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,7 +1684,7 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,7 +1692,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1700,7 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,7 +1708,59 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1682,12 +1771,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc: update todo list
</commit_message>
<xml_diff>
--- a/doc/doc_todo.xlsx
+++ b/doc/doc_todo.xlsx
@@ -12,12 +12,11 @@
     <sheet name="concerns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="142">
   <si>
     <t>file</t>
   </si>
@@ -1553,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,6 +1758,9 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
       <c r="C36" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
doc: todo list update
</commit_message>
<xml_diff>
--- a/doc/doc_todo.xlsx
+++ b/doc/doc_todo.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="7215" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="7215" windowHeight="8130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="asis" sheetId="1" r:id="rId1"/>
     <sheet name="todo" sheetId="2" r:id="rId2"/>
-    <sheet name="concerns" sheetId="3" r:id="rId3"/>
+    <sheet name="list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="204">
   <si>
     <t>file</t>
   </si>
@@ -417,12 +417,6 @@
     <t>tests/test_data.py passes</t>
   </si>
   <si>
-    <t>module</t>
-  </si>
-  <si>
-    <t>concern</t>
-  </si>
-  <si>
     <t xml:space="preserve">fit.fit_consistent &lt;- fit_model.fit_consistent_model </t>
   </si>
   <si>
@@ -442,6 +436,198 @@
   </si>
   <si>
     <t>delete data_model.py</t>
+  </si>
+  <si>
+    <t>ism.consistent &lt;- consistent_model.consistent_model</t>
+  </si>
+  <si>
+    <t>delete consistent_model</t>
+  </si>
+  <si>
+    <t>refactor to ism.age_specific_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_pattern.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: fix AdaptiveMetropolis so that this is not necessary</t>
+  </si>
+  <si>
+    <t>age_pattern.py:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: change old code to use new name, remove this legacy function name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covariate_model.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> add sex as a fixed effect (TODO: decide if this should be in data.py, when loading gbd model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: refactor to reduce duplicate code (this is very similar to code for alpha above)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covariate_model.py:            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: implement a more robust way to align alpha_trace and U_l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.py:                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: eliminate unnecessary dichotomy in storing fe and re priors separately</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.py:        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: refactor prediction code from covariate_model.py into ism.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: catch _csv.Error and retry, to give j drive time to sync</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.py:            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.input_data.dtypes[field] = float  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: figure out classy way like this, that works</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: figure out where negative values could come from in CODEm db</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: test cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: make these vary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit_posterior.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: check for missing covariates, and have them fixed, instead of filling them with zeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit_posterior.py:            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: determine best way to propagate prior on function</t>
+  </si>
+  <si>
+    <t>fit.py:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: move fit_model.fit_consistent_model to fit.fit_consistent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good_dense_data.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO:  take age structure from real data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good_dense_data.py:                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: use this approach to age standardize all gold data, and then change it to get iX as a direct sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: find or set the model number for this model, set the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ism.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: expose (and document) interface for alternative rate_type as well as other options,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ism.py:            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: allow options for alternative priors for sigma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: refactor the way priors are handled</t>
+  </si>
+  <si>
+    <t>ism.py:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: refactor emp_priors into a class and document them</t>
+  </si>
+  <si>
+    <t>Matplot.py:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: make sure pair_posterior works.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pand3.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: check that groupby appears and there are not too many groups</t>
+  </si>
+  <si>
+    <t>rate_model.py:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: remove this legacy-named method</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: save delta in these files, use negative binomial to calc logp</t>
+  </si>
+  <si>
+    <t>dir = dismod3.settings.JOB_WORKING_DIR % id   TODO: refactor into a function</t>
+  </si>
+  <si>
+    <t>dir = dismod3.settings.JOB_WORKING_DIR % id  TODO: refactor into a function</t>
+  </si>
+  <si>
+    <t>fit_all.py:</t>
+  </si>
+  <si>
+    <t>download_model.py:</t>
+  </si>
+  <si>
+    <t>data_simulation.py:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.py:                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iso3 = 'TWN'   TODO: average over CHN, PRK, TWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.py:                                            </t>
+  </si>
+  <si>
+    <t>iso3 = 'CUB'  TODO: average over caribbean countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if isinstance(mu_age_parent, mc.Node):  TODO: test this code</t>
+  </si>
+  <si>
+    <t>age_weights = pl.ones_like(vars['mu_age'].value)  TODO: use age pattern appropriate to the rate type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pand3.py:            </t>
+  </si>
+  <si>
+    <t>assert col in df, 'Column "%s" not found in DataFrame' % col   TODO: say which param has the bad col name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refit_missing.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">upload_fits.py:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TODO: save ref values </t>
   </si>
 </sst>
 </file>
@@ -465,7 +651,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +667,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -528,6 +726,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,8 +1032,8 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1277,7 @@
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G26" t="s">
@@ -1460,8 +1660,11 @@
       <c r="B75" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C75" t="s">
-        <v>14</v>
+      <c r="F75" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,7 +1674,7 @@
       <c r="B77" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F77" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G77" t="s">
@@ -1550,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1926,7 @@
         <v>120</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1731,22 +1934,22 @@
         <v>120</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1754,7 +1957,7 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1762,7 +1965,31 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1773,23 +2000,319 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>134</v>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc todo list updates
</commit_message>
<xml_diff>
--- a/doc/doc_todo.xlsx
+++ b/doc/doc_todo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="7215" windowHeight="8130" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="7215" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="asis" sheetId="1" r:id="rId1"/>
@@ -1031,9 +1031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,318 +2000,318 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="B1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>147</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>154</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>195</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>192</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>191</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>190</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>163</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>165</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>167</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>169</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>171</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>169</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>174</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>176</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>174</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>176</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>174</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>179</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>181</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>199</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>183</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>185</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>201</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>201</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>202</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>202</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>